<commit_message>
Coke Cooler Purity scene/session hierarchy fully established and working
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS_SAND/CMA/Data/CMA Compliance Template v0.9.xlsx
+++ b/Projects/CCBOTTLERSUS_SAND/CMA/Data/CMA Compliance Template v0.9.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="48">
   <si>
     <t xml:space="preserve">KPI name</t>
   </si>
@@ -157,34 +157,10 @@
     <t xml:space="preserve">target</t>
   </si>
   <si>
-    <t xml:space="preserve">SOS SSD</t>
-  </si>
-  <si>
     <t xml:space="preserve">UNITED</t>
   </si>
   <si>
     <t xml:space="preserve">Baton Rouge Preferred</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOS Still</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOS Isotonic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOS Tea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOS Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOS Energy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOS Juice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOS Enhanced Water (Vitamin Water)</t>
   </si>
   <si>
     <t xml:space="preserve">Baton Rouge Partnership</t>
@@ -487,10 +463,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1012145748988"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.8137651821862"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1781376518219"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -654,7 +630,7 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="4" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="47.9878542510121"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="48.417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="4" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1013" min="4" style="4" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1022" min="1014" style="5" width="9.10526315789474"/>
@@ -701,23 +677,23 @@
   </sheetPr>
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.8866396761134"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="28.1740890688259"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="28.3846153846154"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -980,15 +956,15 @@
   </sheetPr>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1012145748988"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
@@ -1012,13 +988,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>46</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>10</v>
@@ -1029,13 +1005,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>46</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>10</v>
@@ -1046,13 +1022,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>46</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>10</v>
@@ -1063,13 +1039,13 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>46</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>10</v>
@@ -1080,13 +1056,13 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>46</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>10</v>
@@ -1097,13 +1073,13 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>46</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>10</v>
@@ -1114,13 +1090,13 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>46</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>10</v>
@@ -1131,13 +1107,13 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>46</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>10</v>
@@ -1148,13 +1124,13 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>10</v>
@@ -1165,13 +1141,13 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>10</v>
@@ -1182,13 +1158,13 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>10</v>
@@ -1199,13 +1175,13 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>10</v>
@@ -1216,13 +1192,13 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>10</v>
@@ -1233,13 +1209,13 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>10</v>
@@ -1250,13 +1226,13 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>10</v>
@@ -1267,13 +1243,13 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>10</v>
@@ -1284,13 +1260,13 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>10</v>
@@ -1301,13 +1277,13 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>47</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>55</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>10</v>
@@ -1318,13 +1294,13 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>10</v>
@@ -1335,13 +1311,13 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>10</v>
@@ -1352,13 +1328,13 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>10</v>
@@ -1369,13 +1345,13 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>10</v>
@@ -1386,13 +1362,13 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>10</v>
@@ -1403,13 +1379,13 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>10</v>

</xml_diff>